<commit_message>
added rule for json and tsv format
</commit_message>
<xml_diff>
--- a/src/test/data/all_data/bpbs_test_ok.xlsx
+++ b/src/test/data/all_data/bpbs_test_ok.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoko/DDBJ/test/data/biosample/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoko/DDBJ/ddbj_validator/src/test/data/all_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C904DDB-12D8-BD41-9AD8-C518E73DA829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65503C96-6205-A145-948F-22E7A4161DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5600" yWindow="1580" windowWidth="27500" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="185">
   <si>
     <t># Submission</t>
   </si>
@@ -553,10 +553,6 @@
   </si>
   <si>
     <t>bio_material</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>oxy_stat_samp</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1076,7 +1072,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1089,7 +1085,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1097,7 +1093,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1105,7 +1101,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1113,7 +1109,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1136,7 +1132,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1144,7 +1140,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1168,7 +1164,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1176,7 +1172,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1209,7 +1205,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1298,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:DB2"/>
+  <dimension ref="A1:DA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="16"/>
@@ -1326,82 +1322,82 @@
     <col min="20" max="20" width="8.42578125" style="8" customWidth="1"/>
     <col min="21" max="21" width="42.85546875" style="8" customWidth="1"/>
     <col min="22" max="22" width="8.42578125" style="8" customWidth="1"/>
-    <col min="23" max="27" width="20" style="8" customWidth="1"/>
-    <col min="28" max="28" width="12" style="8" customWidth="1"/>
-    <col min="29" max="29" width="16.85546875" style="8" customWidth="1"/>
-    <col min="30" max="30" width="9.5703125" style="8" customWidth="1"/>
-    <col min="31" max="31" width="15.5703125" style="8" customWidth="1"/>
-    <col min="32" max="32" width="9.5703125" style="8" customWidth="1"/>
-    <col min="33" max="33" width="21.5703125" style="8" customWidth="1"/>
-    <col min="34" max="34" width="8.42578125" style="8" customWidth="1"/>
-    <col min="35" max="35" width="22.85546875" style="8" customWidth="1"/>
-    <col min="36" max="36" width="16.85546875" style="8" customWidth="1"/>
-    <col min="37" max="38" width="8.42578125" style="8" customWidth="1"/>
-    <col min="39" max="39" width="19.140625" style="8" customWidth="1"/>
-    <col min="40" max="40" width="22.85546875" style="8" customWidth="1"/>
-    <col min="41" max="41" width="9.5703125" style="8" customWidth="1"/>
-    <col min="42" max="42" width="13.140625" style="8" customWidth="1"/>
-    <col min="43" max="43" width="16.85546875" style="8" customWidth="1"/>
-    <col min="44" max="44" width="20.42578125" style="8" customWidth="1"/>
-    <col min="45" max="45" width="15.5703125" style="8" customWidth="1"/>
-    <col min="46" max="46" width="18" style="8" customWidth="1"/>
-    <col min="47" max="47" width="15.5703125" style="8" customWidth="1"/>
-    <col min="48" max="48" width="16.85546875" style="8" customWidth="1"/>
-    <col min="49" max="49" width="13.140625" style="8" customWidth="1"/>
-    <col min="50" max="51" width="16.85546875" style="8" customWidth="1"/>
-    <col min="52" max="52" width="22.85546875" style="8" customWidth="1"/>
-    <col min="53" max="53" width="18" style="8" customWidth="1"/>
-    <col min="54" max="54" width="14.42578125" style="8" customWidth="1"/>
-    <col min="55" max="55" width="12" style="8" customWidth="1"/>
-    <col min="56" max="56" width="19.140625" style="8" customWidth="1"/>
-    <col min="57" max="57" width="10.85546875" style="8" customWidth="1"/>
-    <col min="58" max="58" width="16.85546875" style="8" customWidth="1"/>
-    <col min="59" max="59" width="22.85546875" style="8" customWidth="1"/>
-    <col min="60" max="60" width="8.42578125" style="8" customWidth="1"/>
-    <col min="61" max="61" width="12" style="8" customWidth="1"/>
-    <col min="62" max="62" width="10.85546875" style="8" customWidth="1"/>
-    <col min="63" max="64" width="8.42578125" style="8" customWidth="1"/>
-    <col min="65" max="65" width="6" style="8" customWidth="1"/>
-    <col min="66" max="66" width="18" style="8" customWidth="1"/>
-    <col min="67" max="67" width="9.5703125" style="8" customWidth="1"/>
-    <col min="68" max="68" width="12" style="8" customWidth="1"/>
-    <col min="69" max="69" width="10.85546875" style="8" customWidth="1"/>
-    <col min="70" max="70" width="16.85546875" style="8" customWidth="1"/>
-    <col min="71" max="73" width="15.5703125" style="8" customWidth="1"/>
-    <col min="74" max="74" width="14.42578125" style="8" customWidth="1"/>
-    <col min="75" max="75" width="22.85546875" style="8" customWidth="1"/>
-    <col min="76" max="76" width="2.42578125" style="8" customWidth="1"/>
-    <col min="77" max="77" width="15.5703125" style="8" customWidth="1"/>
-    <col min="78" max="78" width="10.85546875" style="8" customWidth="1"/>
-    <col min="79" max="79" width="24" style="8" customWidth="1"/>
-    <col min="80" max="80" width="10.85546875" style="8" customWidth="1"/>
-    <col min="81" max="81" width="9.5703125" style="8" customWidth="1"/>
-    <col min="82" max="82" width="18" style="8" customWidth="1"/>
-    <col min="83" max="83" width="15.5703125" style="8" customWidth="1"/>
-    <col min="84" max="84" width="9.5703125" style="8" customWidth="1"/>
-    <col min="85" max="85" width="22.85546875" style="8" customWidth="1"/>
-    <col min="86" max="86" width="19.140625" style="8" customWidth="1"/>
-    <col min="87" max="87" width="10.85546875" style="8" customWidth="1"/>
-    <col min="88" max="89" width="16.85546875" style="8" customWidth="1"/>
-    <col min="90" max="90" width="18" style="8" customWidth="1"/>
-    <col min="91" max="91" width="22.85546875" style="8" customWidth="1"/>
-    <col min="92" max="92" width="9.5703125" style="8" customWidth="1"/>
-    <col min="93" max="93" width="7.140625" style="8" customWidth="1"/>
-    <col min="94" max="94" width="21.5703125" style="8" customWidth="1"/>
-    <col min="95" max="95" width="19.140625" style="8" customWidth="1"/>
-    <col min="96" max="97" width="8.42578125" style="8" customWidth="1"/>
-    <col min="98" max="98" width="4.85546875" style="8" customWidth="1"/>
-    <col min="99" max="99" width="9.5703125" style="8" customWidth="1"/>
-    <col min="100" max="100" width="10.85546875" style="8" customWidth="1"/>
-    <col min="101" max="101" width="14.42578125" style="8" customWidth="1"/>
-    <col min="102" max="102" width="15.5703125" style="8" customWidth="1"/>
-    <col min="103" max="103" width="10.85546875" style="8" customWidth="1"/>
-    <col min="104" max="104" width="15.5703125" style="8" customWidth="1"/>
-    <col min="105" max="106" width="13" style="8" customWidth="1"/>
-    <col min="107" max="16384" width="14.42578125" style="7"/>
+    <col min="23" max="26" width="20" style="8" customWidth="1"/>
+    <col min="27" max="27" width="12" style="8" customWidth="1"/>
+    <col min="28" max="28" width="16.85546875" style="8" customWidth="1"/>
+    <col min="29" max="29" width="9.5703125" style="8" customWidth="1"/>
+    <col min="30" max="30" width="15.5703125" style="8" customWidth="1"/>
+    <col min="31" max="31" width="9.5703125" style="8" customWidth="1"/>
+    <col min="32" max="32" width="21.5703125" style="8" customWidth="1"/>
+    <col min="33" max="33" width="8.42578125" style="8" customWidth="1"/>
+    <col min="34" max="34" width="22.85546875" style="8" customWidth="1"/>
+    <col min="35" max="35" width="16.85546875" style="8" customWidth="1"/>
+    <col min="36" max="37" width="8.42578125" style="8" customWidth="1"/>
+    <col min="38" max="38" width="19.140625" style="8" customWidth="1"/>
+    <col min="39" max="39" width="22.85546875" style="8" customWidth="1"/>
+    <col min="40" max="40" width="9.5703125" style="8" customWidth="1"/>
+    <col min="41" max="41" width="13.140625" style="8" customWidth="1"/>
+    <col min="42" max="42" width="16.85546875" style="8" customWidth="1"/>
+    <col min="43" max="43" width="20.42578125" style="8" customWidth="1"/>
+    <col min="44" max="44" width="15.5703125" style="8" customWidth="1"/>
+    <col min="45" max="45" width="18" style="8" customWidth="1"/>
+    <col min="46" max="46" width="15.5703125" style="8" customWidth="1"/>
+    <col min="47" max="47" width="16.85546875" style="8" customWidth="1"/>
+    <col min="48" max="48" width="13.140625" style="8" customWidth="1"/>
+    <col min="49" max="50" width="16.85546875" style="8" customWidth="1"/>
+    <col min="51" max="51" width="22.85546875" style="8" customWidth="1"/>
+    <col min="52" max="52" width="18" style="8" customWidth="1"/>
+    <col min="53" max="53" width="14.42578125" style="8" customWidth="1"/>
+    <col min="54" max="54" width="12" style="8" customWidth="1"/>
+    <col min="55" max="55" width="19.140625" style="8" customWidth="1"/>
+    <col min="56" max="56" width="10.85546875" style="8" customWidth="1"/>
+    <col min="57" max="57" width="16.85546875" style="8" customWidth="1"/>
+    <col min="58" max="58" width="22.85546875" style="8" customWidth="1"/>
+    <col min="59" max="59" width="8.42578125" style="8" customWidth="1"/>
+    <col min="60" max="60" width="12" style="8" customWidth="1"/>
+    <col min="61" max="61" width="10.85546875" style="8" customWidth="1"/>
+    <col min="62" max="63" width="8.42578125" style="8" customWidth="1"/>
+    <col min="64" max="64" width="6" style="8" customWidth="1"/>
+    <col min="65" max="65" width="18" style="8" customWidth="1"/>
+    <col min="66" max="66" width="9.5703125" style="8" customWidth="1"/>
+    <col min="67" max="67" width="12" style="8" customWidth="1"/>
+    <col min="68" max="68" width="10.85546875" style="8" customWidth="1"/>
+    <col min="69" max="69" width="16.85546875" style="8" customWidth="1"/>
+    <col min="70" max="72" width="15.5703125" style="8" customWidth="1"/>
+    <col min="73" max="73" width="14.42578125" style="8" customWidth="1"/>
+    <col min="74" max="74" width="22.85546875" style="8" customWidth="1"/>
+    <col min="75" max="75" width="2.42578125" style="8" customWidth="1"/>
+    <col min="76" max="76" width="15.5703125" style="8" customWidth="1"/>
+    <col min="77" max="77" width="10.85546875" style="8" customWidth="1"/>
+    <col min="78" max="78" width="24" style="8" customWidth="1"/>
+    <col min="79" max="79" width="10.85546875" style="8" customWidth="1"/>
+    <col min="80" max="80" width="9.5703125" style="8" customWidth="1"/>
+    <col min="81" max="81" width="18" style="8" customWidth="1"/>
+    <col min="82" max="82" width="15.5703125" style="8" customWidth="1"/>
+    <col min="83" max="83" width="9.5703125" style="8" customWidth="1"/>
+    <col min="84" max="84" width="22.85546875" style="8" customWidth="1"/>
+    <col min="85" max="85" width="19.140625" style="8" customWidth="1"/>
+    <col min="86" max="86" width="10.85546875" style="8" customWidth="1"/>
+    <col min="87" max="88" width="16.85546875" style="8" customWidth="1"/>
+    <col min="89" max="89" width="18" style="8" customWidth="1"/>
+    <col min="90" max="90" width="22.85546875" style="8" customWidth="1"/>
+    <col min="91" max="91" width="9.5703125" style="8" customWidth="1"/>
+    <col min="92" max="92" width="7.140625" style="8" customWidth="1"/>
+    <col min="93" max="93" width="21.5703125" style="8" customWidth="1"/>
+    <col min="94" max="94" width="19.140625" style="8" customWidth="1"/>
+    <col min="95" max="96" width="8.42578125" style="8" customWidth="1"/>
+    <col min="97" max="97" width="4.85546875" style="8" customWidth="1"/>
+    <col min="98" max="98" width="9.5703125" style="8" customWidth="1"/>
+    <col min="99" max="99" width="10.85546875" style="8" customWidth="1"/>
+    <col min="100" max="100" width="14.42578125" style="8" customWidth="1"/>
+    <col min="101" max="101" width="15.5703125" style="8" customWidth="1"/>
+    <col min="102" max="102" width="10.85546875" style="8" customWidth="1"/>
+    <col min="103" max="103" width="15.5703125" style="8" customWidth="1"/>
+    <col min="104" max="105" width="13" style="8" customWidth="1"/>
+    <col min="106" max="16384" width="14.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:106">
+    <row r="1" spans="1:105">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>
@@ -1481,243 +1477,240 @@
         <v>168</v>
       </c>
       <c r="AA1" s="10" t="s">
-        <v>169</v>
+        <v>50</v>
       </c>
       <c r="AB1" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AC1" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AD1" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AE1" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AF1" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AG1" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AH1" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AI1" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AJ1" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK1" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AL1" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AM1" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AN1" s="10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AO1" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AP1" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AQ1" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AR1" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AS1" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AT1" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AU1" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AV1" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AW1" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AX1" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AY1" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AZ1" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="BA1" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="BB1" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="BC1" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="BD1" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="BE1" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="BF1" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="BG1" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="BH1" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="BI1" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="BJ1" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="BK1" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="BL1" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BM1" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="BN1" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="BO1" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="BP1" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="BQ1" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BR1" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="BS1" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="BT1" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="BU1" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BV1" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="BW1" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="BX1" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="BY1" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="BZ1" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="CA1" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="CB1" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="CC1" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="CD1" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="CE1" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="CF1" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="CG1" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="CH1" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="CI1" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="CJ1" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="CK1" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="CL1" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="CM1" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="CN1" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="CO1" s="10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="CP1" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="CQ1" s="10" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="CR1" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="CS1" s="10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="CT1" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="CU1" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="CV1" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="CW1" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="CX1" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="CY1" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="CZ1" s="10" t="s">
         <v>126</v>
       </c>
+      <c r="CZ1" s="10"/>
       <c r="DA1" s="10"/>
-      <c r="DB1" s="10"/>
-    </row>
-    <row r="2" spans="1:106">
+    </row>
+    <row r="2" spans="1:105">
       <c r="A2" s="11" t="s">
         <v>127</v>
       </c>
@@ -1728,13 +1721,13 @@
         <v>155</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>179</v>
-      </c>
       <c r="I2" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>157</v>
@@ -1752,19 +1745,19 @@
         <v>159</v>
       </c>
       <c r="O2" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="P2" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="Q2" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="R2" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="Q2" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="R2" s="8" t="s">
+      <c r="S2" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>183</v>
       </c>
       <c r="T2" s="8" t="s">
         <v>163</v>

</xml_diff>